<commit_message>
Made all form display flex and made correction on styling.
</commit_message>
<xml_diff>
--- a/inventory/xlsx_for_testing/template__3.xlsx
+++ b/inventory/xlsx_for_testing/template__3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pythonProjects\Inventory\xlsx_for_testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pythonProjects\Inventory\inventory\xlsx_for_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFBECE1-AE15-4FC8-A21A-9002445D34F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287569F6-F95A-4A9A-9EA4-E2637098D89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40872" yWindow="-1188" windowWidth="22176" windowHeight="15348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>